<commit_message>
correção da planilha e sprints
</commit_message>
<xml_diff>
--- a/Sprints/all sprint's.xlsx
+++ b/Sprints/all sprint's.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\PIM\Sprints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WIND10\Desktop\PIM\Sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D31A4F5-2C4B-4268-BDF3-CB78E60CA572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756BC12D-20D6-4D85-97A6-80BB069321D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30930" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{81DB2150-C026-4321-8957-A526B703828E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{81DB2150-C026-4321-8957-A526B703828E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprints" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="82">
   <si>
     <t>SPRINT</t>
   </si>
@@ -220,13 +218,73 @@
   </si>
   <si>
     <t>Edições nos Diagramas</t>
+  </si>
+  <si>
+    <t>2 Horas</t>
+  </si>
+  <si>
+    <t>1 Hora</t>
+  </si>
+  <si>
+    <t>1 Hora e 50 Minutos</t>
+  </si>
+  <si>
+    <t>50 Minutos</t>
+  </si>
+  <si>
+    <t>1 Hora e 10 Minutos</t>
+  </si>
+  <si>
+    <t>1 Horas e 30 Minutos</t>
+  </si>
+  <si>
+    <t>1 Hora e 30 Minutos</t>
+  </si>
+  <si>
+    <t>1 Hora e 40 Minutos</t>
+  </si>
+  <si>
+    <t>RESULTADO EM HORAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 Horas e 20 Minutos</t>
+  </si>
+  <si>
+    <t>2 Horas e 15 Minutos</t>
+  </si>
+  <si>
+    <t>2 Horas 30 Minutos</t>
+  </si>
+  <si>
+    <t>1 Hora e 15 Minutos</t>
+  </si>
+  <si>
+    <t>35 Minutos</t>
+  </si>
+  <si>
+    <t>1 Hora e 25 Minutos</t>
+  </si>
+  <si>
+    <t>1 Hora e 45 Minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1 Hora e 50Minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 Hora e 40 Minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 Hora e 30 Minutos</t>
+  </si>
+  <si>
+    <t>1 Hora 20 Minutos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +296,12 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -324,7 +388,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -452,14 +535,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D163B49-7BC9-465F-AF34-1A102F320B3C}" name="Tabela1" displayName="Tabela1" ref="B2:F40" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="B2:F40" xr:uid="{6D163B49-7BC9-465F-AF34-1A102F320B3C}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2C9AEE50-7AE4-43EA-8B3D-46D9E1CAF5D8}" name="SPRINT" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{947D6CA3-DD72-4E8C-8EDA-5E058A866723}" name="DATA" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{A307DDD7-B6BE-4B10-A582-2C6F9541972C}" name="TAREFA" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{62CE9A6F-DAE5-442B-8C06-3D3B277F701E}" name="QUEM REALIZOU" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{F346D52B-FACA-4F75-8A28-D9896F3A05DE}" name="STATUS" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D163B49-7BC9-465F-AF34-1A102F320B3C}" name="Tabela1" displayName="Tabela1" ref="B2:G39" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B2:G39" xr:uid="{6D163B49-7BC9-465F-AF34-1A102F320B3C}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{2C9AEE50-7AE4-43EA-8B3D-46D9E1CAF5D8}" name="SPRINT" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{947D6CA3-DD72-4E8C-8EDA-5E058A866723}" name="DATA" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{A307DDD7-B6BE-4B10-A582-2C6F9541972C}" name="TAREFA" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{62CE9A6F-DAE5-442B-8C06-3D3B277F701E}" name="QUEM REALIZOU" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{A222EFD4-9FD6-4BF0-A33B-50258BB157E0}" name="RESULTADO EM HORAS" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{F346D52B-FACA-4F75-8A28-D9896F3A05DE}" name="STATUS" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -762,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEC6B00-DAFC-43DC-9B0E-5E08A44B945E}">
-  <dimension ref="B1:F40"/>
+  <dimension ref="B1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,11 +859,12 @@
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="58.7109375" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -793,10 +878,13 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -810,10 +898,13 @@
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -827,17 +918,21 @@
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
@@ -851,10 +946,13 @@
         <v>14</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
@@ -868,10 +966,13 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
@@ -885,17 +986,21 @@
         <v>18</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
@@ -909,10 +1014,13 @@
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
@@ -926,10 +1034,13 @@
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
@@ -943,17 +1054,21 @@
         <v>8</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
@@ -967,10 +1082,13 @@
         <v>11</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -984,10 +1102,13 @@
         <v>28</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1001,17 +1122,21 @@
         <v>8</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>30</v>
       </c>
@@ -1025,10 +1150,13 @@
         <v>33</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>30</v>
       </c>
@@ -1042,10 +1170,13 @@
         <v>11</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
@@ -1059,17 +1190,21 @@
         <v>28</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>36</v>
       </c>
@@ -1083,10 +1218,13 @@
         <v>8</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>36</v>
       </c>
@@ -1100,10 +1238,13 @@
         <v>8</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>36</v>
       </c>
@@ -1117,10 +1258,13 @@
         <v>16</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>36</v>
       </c>
@@ -1133,18 +1277,22 @@
       <c r="E25" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>42</v>
       </c>
@@ -1157,11 +1305,14 @@
       <c r="E27" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>42</v>
       </c>
@@ -1175,10 +1326,13 @@
         <v>33</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>42</v>
       </c>
@@ -1192,10 +1346,13 @@
         <v>16</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>42</v>
       </c>
@@ -1208,11 +1365,14 @@
       <c r="E30" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>42</v>
       </c>
@@ -1226,17 +1386,21 @@
         <v>51</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>58</v>
       </c>
@@ -1250,10 +1414,13 @@
         <v>57</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>58</v>
       </c>
@@ -1267,10 +1434,13 @@
         <v>51</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>58</v>
       </c>
@@ -1284,10 +1454,13 @@
         <v>16</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>58</v>
       </c>
@@ -1301,10 +1474,13 @@
         <v>56</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>58</v>
       </c>
@@ -1317,11 +1493,14 @@
       <c r="E37" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>58</v>
       </c>
@@ -1335,10 +1514,13 @@
         <v>28</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>58</v>
       </c>
@@ -1352,17 +1534,14 @@
         <v>28</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
+        <v>68</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>